<commit_message>
Implemented adding data to sheet (numbers and strings)
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -13,6 +13,14 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>test</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,12 +350,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>